<commit_message>
changes instance vm size of windows machines, use windows server 2016 datacenter, since core does not seem available.
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/aws_app_invoice.xlsx
+++ b/src/regionify/invoices/aws_app_invoice.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="0" windowWidth="24000" windowHeight="9030"/>
+    <workbookView xWindow="7680" yWindow="0" windowWidth="24000" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,20 +129,20 @@
     <t>t2.nano</t>
   </si>
   <si>
-    <t>Centos 7</t>
-  </si>
-  <si>
     <t>Ubuntu 14</t>
   </si>
   <si>
     <t>RHEL 7</t>
+  </si>
+  <si>
+    <t>CentOS 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +170,12 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -199,6 +205,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +525,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,11 +576,11 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>33</v>
@@ -600,10 +609,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>33</v>
@@ -623,10 +632,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
install type for rhel changed to t1.micro
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/aws_app_invoice.xlsx
+++ b/src/regionify/invoices/aws_app_invoice.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>OS</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>CentOS 7</t>
+  </si>
+  <si>
+    <t>t2.micro</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +618,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
instance size of rhel to t2.micro
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/aws_app_invoice.xlsx
+++ b/src/regionify/invoices/aws_app_invoice.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>OS</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>CentOS 7</t>
+  </si>
+  <si>
+    <t>t2.micro</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +618,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
fixed ami_id for ubuntu 14 on aws
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/aws_app_invoice.xlsx
+++ b/src/regionify/invoices/aws_app_invoice.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>OS</t>
   </si>
@@ -108,21 +108,6 @@
     <t>ami-8cff51fb</t>
   </si>
   <si>
-    <t>ami-2d57433a</t>
-  </si>
-  <si>
-    <t>ami-e7277687</t>
-  </si>
-  <si>
-    <t>ami-900ebaf0</t>
-  </si>
-  <si>
-    <t>ami-75c9e906</t>
-  </si>
-  <si>
-    <t>ami-162ded79</t>
-  </si>
-  <si>
     <t>Instance Type</t>
   </si>
   <si>
@@ -139,6 +124,18 @@
   </si>
   <si>
     <t>t2.micro</t>
+  </si>
+  <si>
+    <t>ami-cfa100d9</t>
+  </si>
+  <si>
+    <t>ami-29752c49</t>
+  </si>
+  <si>
+    <t>ami-32517b54</t>
+  </si>
+  <si>
+    <t>ami-0738ec68</t>
   </si>
 </sst>
 </file>
@@ -528,7 +525,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>15</v>
@@ -580,13 +577,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -612,13 +609,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -635,28 +632,25 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed ubuntu ami-ids for aws
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/aws_app_invoice.xlsx
+++ b/src/regionify/invoices/aws_app_invoice.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>OS</t>
   </si>
@@ -108,21 +108,6 @@
     <t>ami-8cff51fb</t>
   </si>
   <si>
-    <t>ami-2d57433a</t>
-  </si>
-  <si>
-    <t>ami-e7277687</t>
-  </si>
-  <si>
-    <t>ami-900ebaf0</t>
-  </si>
-  <si>
-    <t>ami-75c9e906</t>
-  </si>
-  <si>
-    <t>ami-162ded79</t>
-  </si>
-  <si>
     <t>Instance Type</t>
   </si>
   <si>
@@ -139,6 +124,24 @@
   </si>
   <si>
     <t>t2.micro</t>
+  </si>
+  <si>
+    <t>ami-9dde7f8b</t>
+  </si>
+  <si>
+    <t>ami-9d772efd</t>
+  </si>
+  <si>
+    <t>ami-0e2aa66e</t>
+  </si>
+  <si>
+    <t>ami-115d7777</t>
+  </si>
+  <si>
+    <t>ami-6039ed0f</t>
+  </si>
+  <si>
+    <t>ami-c29184a6</t>
   </si>
 </sst>
 </file>
@@ -528,7 +531,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>15</v>
@@ -580,13 +583,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -612,13 +615,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -635,28 +638,31 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed ubuntu amiids for aws
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/aws_app_invoice.xlsx
+++ b/src/regionify/invoices/aws_app_invoice.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>OS</t>
   </si>
@@ -126,16 +126,22 @@
     <t>t2.micro</t>
   </si>
   <si>
-    <t>ami-cfa100d9</t>
-  </si>
-  <si>
-    <t>ami-29752c49</t>
-  </si>
-  <si>
-    <t>ami-32517b54</t>
-  </si>
-  <si>
-    <t>ami-0738ec68</t>
+    <t>ami-9dde7f8b</t>
+  </si>
+  <si>
+    <t>ami-9d772efd</t>
+  </si>
+  <si>
+    <t>ami-0e2aa66e</t>
+  </si>
+  <si>
+    <t>ami-115d7777</t>
+  </si>
+  <si>
+    <t>ami-6039ed0f</t>
+  </si>
+  <si>
+    <t>ami-c29184a6</t>
   </si>
 </sst>
 </file>
@@ -525,7 +531,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,11 +652,17 @@
       <c r="F4" t="s">
         <v>34</v>
       </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed ubuntu ami ids for aws
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/aws_app_invoice.xlsx
+++ b/src/regionify/invoices/aws_app_invoice.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>OS</t>
   </si>
@@ -108,21 +108,6 @@
     <t>ami-8cff51fb</t>
   </si>
   <si>
-    <t>ami-2d57433a</t>
-  </si>
-  <si>
-    <t>ami-e7277687</t>
-  </si>
-  <si>
-    <t>ami-900ebaf0</t>
-  </si>
-  <si>
-    <t>ami-75c9e906</t>
-  </si>
-  <si>
-    <t>ami-162ded79</t>
-  </si>
-  <si>
     <t>Instance Type</t>
   </si>
   <si>
@@ -151,6 +136,24 @@
   </si>
   <si>
     <t>logos\Centos.png</t>
+  </si>
+  <si>
+    <t>ami-9dde7f8b</t>
+  </si>
+  <si>
+    <t>ami-9d772efd</t>
+  </si>
+  <si>
+    <t>ami-0e2aa66e</t>
+  </si>
+  <si>
+    <t>ami-115d7777</t>
+  </si>
+  <si>
+    <t>ami-6039ed0f</t>
+  </si>
+  <si>
+    <t>ami-c29184a6</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
@@ -595,16 +598,16 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -630,16 +633,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -656,31 +659,34 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
         <v>40</v>
       </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated amazon ubuntu14 ami's
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/aws_app_invoice.xlsx
+++ b/src/regionify/invoices/aws_app_invoice.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\preconfigured-apps\src\regionify\invoices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Git\app-starter-pack\src\regionify\invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -138,22 +138,22 @@
     <t>logos\Centos.png</t>
   </si>
   <si>
-    <t>ami-9dde7f8b</t>
-  </si>
-  <si>
-    <t>ami-9d772efd</t>
-  </si>
-  <si>
-    <t>ami-0e2aa66e</t>
-  </si>
-  <si>
-    <t>ami-115d7777</t>
-  </si>
-  <si>
-    <t>ami-6039ed0f</t>
-  </si>
-  <si>
-    <t>ami-c29184a6</t>
+    <t>ami-4a9b1930</t>
+  </si>
+  <si>
+    <t>ami-1d90a97d</t>
+  </si>
+  <si>
+    <t>ami-0fcf1c77</t>
+  </si>
+  <si>
+    <t>ami-308d2749</t>
+  </si>
+  <si>
+    <t>ami-5029a93f</t>
+  </si>
+  <si>
+    <t>ami-3ec8d75a</t>
   </si>
 </sst>
 </file>
@@ -319,23 +319,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -371,23 +354,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -543,7 +509,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>